<commit_message>
updates the rollout to reflect the new PCB ordering deadline
</commit_message>
<xml_diff>
--- a/documentation/ChatterTale Rollout.xlsx
+++ b/documentation/ChatterTale Rollout.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -29,7 +28,7 @@
     <t>Task</t>
   </si>
   <si>
-    <t>Lead Team Member </t>
+    <t>Lead Team Member</t>
   </si>
   <si>
     <t>Secondary</t>
@@ -53,31 +52,31 @@
     <t>Ali</t>
   </si>
   <si>
-    <t>   Order battery (define the battery)</t>
+    <t>Order battery (define the battery)</t>
   </si>
   <si>
     <t>Rodrigo</t>
   </si>
   <si>
-    <t>   Design packaging</t>
-  </si>
-  <si>
-    <t>   Redesign PCB board</t>
-  </si>
-  <si>
-    <t>   Order Stickers</t>
-  </si>
-  <si>
-    <t>   Order PCB board</t>
-  </si>
-  <si>
-    <t>   Define parts (pot, speaker, buttons)</t>
+    <t>Design packaging</t>
+  </si>
+  <si>
+    <t>Redesign PCB board</t>
+  </si>
+  <si>
+    <t>Order Stickers</t>
+  </si>
+  <si>
+    <t>Order PCB board</t>
+  </si>
+  <si>
+    <t>Define parts (pot, speaker, buttons)</t>
   </si>
   <si>
     <t>Coordinate with Library</t>
   </si>
   <si>
-    <t>   Order internal components</t>
+    <t>Order internal components</t>
   </si>
   <si>
     <t>Paapa/Ali</t>
@@ -95,61 +94,61 @@
     <t>Assemble sets of electronics</t>
   </si>
   <si>
-    <t>    Define buttons and how to fix them</t>
-  </si>
-  <si>
-    <t>       Button labeling (stickers? 3D printed symbols?)</t>
-  </si>
-  <si>
-    <t>    Define how to fix the jack </t>
+    <t>Define buttons and how to fix them</t>
+  </si>
+  <si>
+    <t>Button labeling (stickers? 3D printed symbols?)</t>
+  </si>
+  <si>
+    <t>Define how to fix the jack</t>
   </si>
   <si>
     <t>Finish ChatterTale Sets</t>
   </si>
   <si>
-    <t>    Add LED low battery indicator</t>
+    <t>Add LED low battery indicator</t>
   </si>
   <si>
     <t>Rodrigo/Catie</t>
   </si>
   <si>
-    <t>    Add LED power-on indicator</t>
+    <t>Add LED power-on indicator</t>
   </si>
   <si>
     <t>Distribute electronics and 3D file to library(s)</t>
   </si>
   <si>
-    <t>    Define how to fix the PBC boards</t>
-  </si>
-  <si>
-    <t>   Add the volume pot to 3D</t>
-  </si>
-  <si>
-    <t>   Ears – test with microphone</t>
+    <t>Define how to fix the PBC boards</t>
+  </si>
+  <si>
+    <t>Add the volume pot to 3D</t>
+  </si>
+  <si>
+    <t>Ears – test with microphone</t>
   </si>
   <si>
     <t>24-Apr</t>
   </si>
   <si>
-    <t>   Ears – test with audio jack</t>
-  </si>
-  <si>
-    <t>   Sketch dimensions</t>
-  </si>
-  <si>
-    <t>   2D drawing</t>
-  </si>
-  <si>
-    <t>   3D case outside</t>
-  </si>
-  <si>
-    <t>   Case inside</t>
-  </si>
-  <si>
-    <t>   Print bear</t>
-  </si>
-  <si>
-    <t>   Final revision</t>
+    <t>Ears – test with audio jack</t>
+  </si>
+  <si>
+    <t>Sketch dimensions</t>
+  </si>
+  <si>
+    <t>2D drawing</t>
+  </si>
+  <si>
+    <t>3D case outside</t>
+  </si>
+  <si>
+    <t>Case inside</t>
+  </si>
+  <si>
+    <t>Print bear</t>
+  </si>
+  <si>
+    <t>Final revision</t>
   </si>
   <si>
     <t>Instructions for printing</t>
@@ -158,24 +157,20 @@
     <t>Test Prototype</t>
   </si>
   <si>
-    <t>   Coordinate with library</t>
-  </si>
-  <si>
-    <t>   Test run with kids</t>
-  </si>
-  <si>
-    <t>  Assess feedback</t>
+    <t>Coordinate with library</t>
+  </si>
+  <si>
+    <t>Test run with kids</t>
+  </si>
+  <si>
+    <t>Assess feedback</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="D\-MMM"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -184,22 +179,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -207,7 +187,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -220,6 +200,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -230,246 +218,538 @@
     </fill>
   </fills>
   <borders count="10">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
-      <bottom style="thin"/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
-      <top style="thin"/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="40.8777777777778"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="20.9"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="11.4"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="10.8962962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="24.0925925925926"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.8962962962963"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="14.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11"/>
+    <col min="1" max="1" width="40.8984375" style="1"/>
+    <col min="2" max="2" width="20.8984375" style="2"/>
+    <col min="3" max="4" width="11.3984375" style="2"/>
+    <col min="5" max="5" width="10.8984375" style="2"/>
+    <col min="6" max="6" width="11"/>
+    <col min="7" max="7" width="24.09765625" style="1"/>
+    <col min="8" max="8" width="22.8984375"/>
+    <col min="9" max="9" width="14.3984375"/>
+    <col min="10" max="1025" width="11"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="G1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="G2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
       <c r="G3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -498,7 +778,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="7"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -509,7 +789,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="9"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>9</v>
       </c>
@@ -526,7 +806,7 @@
       <c r="I6" s="11"/>
       <c r="J6" s="12"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
@@ -534,7 +814,7 @@
         <v>13</v>
       </c>
       <c r="C7" s="11"/>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="13">
         <v>42115</v>
       </c>
       <c r="E7" s="12"/>
@@ -547,7 +827,7 @@
       <c r="I7" s="11"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
@@ -555,7 +835,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="11"/>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="13">
         <v>42122</v>
       </c>
       <c r="E8" s="12"/>
@@ -568,7 +848,7 @@
       <c r="I8" s="11"/>
       <c r="J8" s="12"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>17</v>
       </c>
@@ -576,8 +856,8 @@
         <v>13</v>
       </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="13" t="n">
-        <v>42125</v>
+      <c r="D9" s="13">
+        <v>42132</v>
       </c>
       <c r="E9" s="12"/>
       <c r="G9" s="10"/>
@@ -585,7 +865,7 @@
       <c r="I9" s="11"/>
       <c r="J9" s="12"/>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>18</v>
       </c>
@@ -593,7 +873,7 @@
         <v>13</v>
       </c>
       <c r="C10" s="11"/>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="19">
         <v>42115</v>
       </c>
       <c r="E10" s="12"/>
@@ -606,7 +886,7 @@
       <c r="I10" s="11"/>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -614,7 +894,7 @@
         <v>21</v>
       </c>
       <c r="C11" s="11"/>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="13">
         <v>42118</v>
       </c>
       <c r="E11" s="12"/>
@@ -623,7 +903,7 @@
       <c r="I11" s="11"/>
       <c r="J11" s="12"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
@@ -638,7 +918,7 @@
       <c r="I12" s="11"/>
       <c r="J12" s="12"/>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>23</v>
       </c>
@@ -646,7 +926,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="11"/>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="13">
         <v>42139</v>
       </c>
       <c r="E13" s="12"/>
@@ -659,7 +939,7 @@
       <c r="I13" s="11"/>
       <c r="J13" s="12"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>26</v>
       </c>
@@ -674,7 +954,7 @@
       <c r="I14" s="11"/>
       <c r="J14" s="12"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>27</v>
       </c>
@@ -682,7 +962,7 @@
         <v>24</v>
       </c>
       <c r="C15" s="11"/>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="13">
         <v>42125</v>
       </c>
       <c r="E15" s="12"/>
@@ -691,7 +971,7 @@
       <c r="I15" s="11"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>28</v>
       </c>
@@ -699,7 +979,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="11"/>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="13">
         <v>42125</v>
       </c>
       <c r="E16" s="12"/>
@@ -707,12 +987,12 @@
         <v>29</v>
       </c>
       <c r="H16" s="11"/>
-      <c r="I16" s="13" t="n">
+      <c r="I16" s="13">
         <v>42156</v>
       </c>
       <c r="J16" s="12"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>30</v>
       </c>
@@ -720,7 +1000,7 @@
         <v>31</v>
       </c>
       <c r="C17" s="11"/>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="13">
         <v>42125</v>
       </c>
       <c r="E17" s="12"/>
@@ -729,7 +1009,7 @@
       <c r="I17" s="11"/>
       <c r="J17" s="12"/>
     </row>
-    <row r="18" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>32</v>
       </c>
@@ -743,12 +1023,12 @@
         <v>33</v>
       </c>
       <c r="H18" s="11"/>
-      <c r="I18" s="13" t="n">
+      <c r="I18" s="13">
         <v>42170</v>
       </c>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>34</v>
       </c>
@@ -763,7 +1043,7 @@
       <c r="I19" s="11"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>35</v>
       </c>
@@ -771,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="C20" s="11"/>
-      <c r="D20" s="13" t="n">
+      <c r="D20" s="13">
         <v>42125</v>
       </c>
       <c r="E20" s="12"/>
@@ -780,7 +1060,7 @@
       <c r="I20" s="11"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>36</v>
       </c>
@@ -797,7 +1077,7 @@
       <c r="I21" s="11"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>38</v>
       </c>
@@ -805,7 +1085,7 @@
         <v>24</v>
       </c>
       <c r="C22" s="11"/>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="13">
         <v>42118</v>
       </c>
       <c r="E22" s="12"/>
@@ -814,7 +1094,7 @@
       <c r="I22" s="11"/>
       <c r="J22" s="12"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>39</v>
       </c>
@@ -822,7 +1102,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="11"/>
-      <c r="D23" s="13" t="n">
+      <c r="D23" s="13">
         <v>42115</v>
       </c>
       <c r="E23" s="12"/>
@@ -831,7 +1111,7 @@
       <c r="I23" s="11"/>
       <c r="J23" s="12"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>40</v>
       </c>
@@ -839,7 +1119,7 @@
         <v>24</v>
       </c>
       <c r="C24" s="11"/>
-      <c r="D24" s="13" t="n">
+      <c r="D24" s="13">
         <v>42118</v>
       </c>
       <c r="E24" s="12"/>
@@ -848,7 +1128,7 @@
       <c r="I24" s="11"/>
       <c r="J24" s="12"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
@@ -856,7 +1136,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="11"/>
-      <c r="D25" s="13" t="n">
+      <c r="D25" s="13">
         <v>42125</v>
       </c>
       <c r="E25" s="12"/>
@@ -865,7 +1145,7 @@
       <c r="I25" s="11"/>
       <c r="J25" s="12"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>42</v>
       </c>
@@ -873,7 +1153,7 @@
         <v>24</v>
       </c>
       <c r="C26" s="11"/>
-      <c r="D26" s="13" t="n">
+      <c r="D26" s="13">
         <v>42132</v>
       </c>
       <c r="E26" s="12"/>
@@ -882,7 +1162,7 @@
       <c r="I26" s="11"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>43</v>
       </c>
@@ -890,7 +1170,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="11"/>
-      <c r="D27" s="13" t="n">
+      <c r="D27" s="13">
         <v>42135</v>
       </c>
       <c r="E27" s="12"/>
@@ -899,7 +1179,7 @@
       <c r="I27" s="11"/>
       <c r="J27" s="12"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>44</v>
       </c>
@@ -907,7 +1187,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="11"/>
-      <c r="D28" s="13" t="n">
+      <c r="D28" s="13">
         <v>42139</v>
       </c>
       <c r="E28" s="12"/>
@@ -916,7 +1196,7 @@
       <c r="I28" s="11"/>
       <c r="J28" s="12"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="11"/>
@@ -927,7 +1207,7 @@
       <c r="I29" s="11"/>
       <c r="J29" s="12"/>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>45</v>
       </c>
@@ -935,7 +1215,7 @@
         <v>24</v>
       </c>
       <c r="C30" s="11"/>
-      <c r="D30" s="13" t="n">
+      <c r="D30" s="13">
         <v>42143</v>
       </c>
       <c r="E30" s="12"/>
@@ -944,7 +1224,7 @@
       <c r="I30" s="11"/>
       <c r="J30" s="12"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -955,7 +1235,7 @@
       <c r="I31" s="11"/>
       <c r="J31" s="12"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>46</v>
       </c>
@@ -968,7 +1248,7 @@
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>47</v>
       </c>
@@ -981,7 +1261,7 @@
       <c r="I33" s="17"/>
       <c r="J33" s="18"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>48</v>
       </c>
@@ -990,7 +1270,7 @@
       <c r="D34" s="11"/>
       <c r="E34" s="12"/>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>49</v>
       </c>
@@ -999,28 +1279,28 @@
       <c r="D35" s="11"/>
       <c r="E35" s="12"/>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11"/>
       <c r="D36" s="11"/>
       <c r="E36" s="12"/>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
       <c r="E37" s="12"/>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="11"/>
       <c r="D38" s="11"/>
       <c r="E38" s="12"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="17"/>
       <c r="C39" s="17"/>
@@ -1028,12 +1308,7 @@
       <c r="E39" s="18"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>